<commit_message>
Fix handling of table properties changes by transformers
The actual fix was implemented in JBehave Core:
https://github.com/vividus-framework/jbehave-core/commit/a88c7a2e6e40e1073efef1b611452f172cfb99a9
</commit_message>
<xml_diff>
--- a/vividus-tests/src/main/resources/data/complex-data.xlsx
+++ b/vividus-tests/src/main/resources/data/complex-data.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10913"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/valery_yatsynovich/work/projects/vividus-framework/vividus/vividus-tests/src/main/resources/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7454F2A-7859-7F40-854E-C337D94BC9F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFEBF766-33B2-224C-BD3B-E3BB0ACCA93B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="480" windowWidth="28800" windowHeight="16660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="480" windowWidth="28800" windowHeight="16660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
+    <sheet name="with separators" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>#</t>
   </si>
@@ -57,6 +58,15 @@
   </si>
   <si>
     <t>Name 3</t>
+  </si>
+  <si>
+    <t>A | B</t>
+  </si>
+  <si>
+    <t>C ! D</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -188,38 +198,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -540,7 +550,7 @@
   </sheetPr>
   <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -551,133 +561,133 @@
     <col min="3" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:2" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2"/>
-    </row>
-    <row r="2" spans="1:2" s="3" customFormat="1" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="B1" s="11"/>
+    </row>
+    <row r="2" spans="1:2" s="2" customFormat="1" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4"/>
-    </row>
-    <row r="3" spans="1:2" s="3" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="B2" s="12"/>
+    </row>
+    <row r="3" spans="1:2" s="2" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="8" customFormat="1" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="6">
+    <row r="4" spans="1:2" s="5" customFormat="1" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="8">
         <v>1</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A5" s="9"/>
-      <c r="B5" s="10"/>
-    </row>
-    <row r="6" spans="1:2" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+      <c r="B5" s="6"/>
+    </row>
+    <row r="6" spans="1:2" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A6" s="9"/>
-      <c r="B6" s="10"/>
-    </row>
-    <row r="7" spans="1:2" s="3" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="6"/>
+    </row>
+    <row r="7" spans="1:2" s="2" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9"/>
-      <c r="B7" s="10"/>
-    </row>
-    <row r="8" spans="1:2" s="3" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="6"/>
+    </row>
+    <row r="8" spans="1:2" s="2" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9"/>
-      <c r="B8" s="10"/>
-    </row>
-    <row r="9" spans="1:2" s="3" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="6"/>
+    </row>
+    <row r="9" spans="1:2" s="2" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9"/>
-      <c r="B9" s="10"/>
-    </row>
-    <row r="10" spans="1:2" s="3" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="6"/>
+    </row>
+    <row r="10" spans="1:2" s="2" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9"/>
-      <c r="B10" s="10"/>
-    </row>
-    <row r="11" spans="1:2" s="3" customFormat="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
-      <c r="B11" s="12"/>
-    </row>
-    <row r="12" spans="1:2" s="8" customFormat="1" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="6">
+      <c r="B10" s="6"/>
+    </row>
+    <row r="11" spans="1:2" s="2" customFormat="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10"/>
+      <c r="B11" s="7"/>
+    </row>
+    <row r="12" spans="1:2" s="5" customFormat="1" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="8">
         <v>2</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:2" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A13" s="9"/>
-      <c r="B13" s="10"/>
-    </row>
-    <row r="14" spans="1:2" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+      <c r="B13" s="6"/>
+    </row>
+    <row r="14" spans="1:2" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A14" s="9"/>
-      <c r="B14" s="10"/>
-    </row>
-    <row r="15" spans="1:2" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+      <c r="B14" s="6"/>
+    </row>
+    <row r="15" spans="1:2" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A15" s="9"/>
-      <c r="B15" s="10"/>
-    </row>
-    <row r="16" spans="1:2" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+      <c r="B15" s="6"/>
+    </row>
+    <row r="16" spans="1:2" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A16" s="9"/>
-      <c r="B16" s="10"/>
-    </row>
-    <row r="17" spans="1:2" s="3" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="6"/>
+    </row>
+    <row r="17" spans="1:2" s="2" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="9"/>
-      <c r="B17" s="10"/>
-    </row>
-    <row r="18" spans="1:2" s="3" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="6"/>
+    </row>
+    <row r="18" spans="1:2" s="2" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="9"/>
-      <c r="B18" s="10"/>
-    </row>
-    <row r="19" spans="1:2" s="3" customFormat="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
-      <c r="B19" s="12"/>
-    </row>
-    <row r="20" spans="1:2" s="8" customFormat="1" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="6">
+      <c r="B18" s="6"/>
+    </row>
+    <row r="19" spans="1:2" s="2" customFormat="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="10"/>
+      <c r="B19" s="7"/>
+    </row>
+    <row r="20" spans="1:2" s="5" customFormat="1" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="8">
         <v>3</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:2" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A21" s="9"/>
-      <c r="B21" s="10"/>
-    </row>
-    <row r="22" spans="1:2" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+      <c r="B21" s="6"/>
+    </row>
+    <row r="22" spans="1:2" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A22" s="9"/>
-      <c r="B22" s="10"/>
-    </row>
-    <row r="23" spans="1:2" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+      <c r="B22" s="6"/>
+    </row>
+    <row r="23" spans="1:2" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A23" s="9"/>
-      <c r="B23" s="10"/>
-    </row>
-    <row r="24" spans="1:2" s="3" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="6"/>
+    </row>
+    <row r="24" spans="1:2" s="2" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="9"/>
-      <c r="B24" s="10"/>
-    </row>
-    <row r="25" spans="1:2" s="3" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="6"/>
+    </row>
+    <row r="25" spans="1:2" s="2" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="9"/>
-      <c r="B25" s="10"/>
-    </row>
-    <row r="26" spans="1:2" s="3" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="6"/>
+    </row>
+    <row r="26" spans="1:2" s="2" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="9"/>
-      <c r="B26" s="10"/>
-    </row>
-    <row r="27" spans="1:2" s="3" customFormat="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="11"/>
-      <c r="B27" s="12"/>
+      <c r="B26" s="6"/>
+    </row>
+    <row r="27" spans="1:2" s="2" customFormat="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="10"/>
+      <c r="B27" s="7"/>
     </row>
     <row r="28" spans="1:2" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
@@ -698,19 +708,50 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54AF4425-696E-FE45-90E4-C765F4779314}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -925,18 +966,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70B6D77D-0519-42E5-8A64-FC8C3D3EB3E2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D06517E-E6DE-43DD-A2B3-44E3324281BB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70B6D77D-0519-42E5-8A64-FC8C3D3EB3E2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Fix handling of table properties changes by transformers (#953)
The actual fix was implemented in JBehave Core:
https://github.com/vividus-framework/jbehave-core/commit/a88c7a2e6e40e1073efef1b611452f172cfb99a9
</commit_message>
<xml_diff>
--- a/vividus-tests/src/main/resources/data/complex-data.xlsx
+++ b/vividus-tests/src/main/resources/data/complex-data.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10913"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/valery_yatsynovich/work/projects/vividus-framework/vividus/vividus-tests/src/main/resources/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7454F2A-7859-7F40-854E-C337D94BC9F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFEBF766-33B2-224C-BD3B-E3BB0ACCA93B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="480" windowWidth="28800" windowHeight="16660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="480" windowWidth="28800" windowHeight="16660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
+    <sheet name="with separators" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>#</t>
   </si>
@@ -57,6 +58,15 @@
   </si>
   <si>
     <t>Name 3</t>
+  </si>
+  <si>
+    <t>A | B</t>
+  </si>
+  <si>
+    <t>C ! D</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -188,38 +198,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -540,7 +550,7 @@
   </sheetPr>
   <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -551,133 +561,133 @@
     <col min="3" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:2" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2"/>
-    </row>
-    <row r="2" spans="1:2" s="3" customFormat="1" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="B1" s="11"/>
+    </row>
+    <row r="2" spans="1:2" s="2" customFormat="1" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4"/>
-    </row>
-    <row r="3" spans="1:2" s="3" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="B2" s="12"/>
+    </row>
+    <row r="3" spans="1:2" s="2" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="8" customFormat="1" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="6">
+    <row r="4" spans="1:2" s="5" customFormat="1" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="8">
         <v>1</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A5" s="9"/>
-      <c r="B5" s="10"/>
-    </row>
-    <row r="6" spans="1:2" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+      <c r="B5" s="6"/>
+    </row>
+    <row r="6" spans="1:2" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A6" s="9"/>
-      <c r="B6" s="10"/>
-    </row>
-    <row r="7" spans="1:2" s="3" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="6"/>
+    </row>
+    <row r="7" spans="1:2" s="2" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9"/>
-      <c r="B7" s="10"/>
-    </row>
-    <row r="8" spans="1:2" s="3" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="6"/>
+    </row>
+    <row r="8" spans="1:2" s="2" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9"/>
-      <c r="B8" s="10"/>
-    </row>
-    <row r="9" spans="1:2" s="3" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="6"/>
+    </row>
+    <row r="9" spans="1:2" s="2" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9"/>
-      <c r="B9" s="10"/>
-    </row>
-    <row r="10" spans="1:2" s="3" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="6"/>
+    </row>
+    <row r="10" spans="1:2" s="2" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9"/>
-      <c r="B10" s="10"/>
-    </row>
-    <row r="11" spans="1:2" s="3" customFormat="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
-      <c r="B11" s="12"/>
-    </row>
-    <row r="12" spans="1:2" s="8" customFormat="1" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="6">
+      <c r="B10" s="6"/>
+    </row>
+    <row r="11" spans="1:2" s="2" customFormat="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10"/>
+      <c r="B11" s="7"/>
+    </row>
+    <row r="12" spans="1:2" s="5" customFormat="1" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="8">
         <v>2</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:2" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A13" s="9"/>
-      <c r="B13" s="10"/>
-    </row>
-    <row r="14" spans="1:2" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+      <c r="B13" s="6"/>
+    </row>
+    <row r="14" spans="1:2" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A14" s="9"/>
-      <c r="B14" s="10"/>
-    </row>
-    <row r="15" spans="1:2" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+      <c r="B14" s="6"/>
+    </row>
+    <row r="15" spans="1:2" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A15" s="9"/>
-      <c r="B15" s="10"/>
-    </row>
-    <row r="16" spans="1:2" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+      <c r="B15" s="6"/>
+    </row>
+    <row r="16" spans="1:2" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A16" s="9"/>
-      <c r="B16" s="10"/>
-    </row>
-    <row r="17" spans="1:2" s="3" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="6"/>
+    </row>
+    <row r="17" spans="1:2" s="2" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="9"/>
-      <c r="B17" s="10"/>
-    </row>
-    <row r="18" spans="1:2" s="3" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="6"/>
+    </row>
+    <row r="18" spans="1:2" s="2" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="9"/>
-      <c r="B18" s="10"/>
-    </row>
-    <row r="19" spans="1:2" s="3" customFormat="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
-      <c r="B19" s="12"/>
-    </row>
-    <row r="20" spans="1:2" s="8" customFormat="1" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="6">
+      <c r="B18" s="6"/>
+    </row>
+    <row r="19" spans="1:2" s="2" customFormat="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="10"/>
+      <c r="B19" s="7"/>
+    </row>
+    <row r="20" spans="1:2" s="5" customFormat="1" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="8">
         <v>3</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:2" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A21" s="9"/>
-      <c r="B21" s="10"/>
-    </row>
-    <row r="22" spans="1:2" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+      <c r="B21" s="6"/>
+    </row>
+    <row r="22" spans="1:2" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A22" s="9"/>
-      <c r="B22" s="10"/>
-    </row>
-    <row r="23" spans="1:2" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+      <c r="B22" s="6"/>
+    </row>
+    <row r="23" spans="1:2" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A23" s="9"/>
-      <c r="B23" s="10"/>
-    </row>
-    <row r="24" spans="1:2" s="3" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="6"/>
+    </row>
+    <row r="24" spans="1:2" s="2" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="9"/>
-      <c r="B24" s="10"/>
-    </row>
-    <row r="25" spans="1:2" s="3" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="6"/>
+    </row>
+    <row r="25" spans="1:2" s="2" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="9"/>
-      <c r="B25" s="10"/>
-    </row>
-    <row r="26" spans="1:2" s="3" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="6"/>
+    </row>
+    <row r="26" spans="1:2" s="2" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="9"/>
-      <c r="B26" s="10"/>
-    </row>
-    <row r="27" spans="1:2" s="3" customFormat="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="11"/>
-      <c r="B27" s="12"/>
+      <c r="B26" s="6"/>
+    </row>
+    <row r="27" spans="1:2" s="2" customFormat="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="10"/>
+      <c r="B27" s="7"/>
     </row>
     <row r="28" spans="1:2" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
@@ -698,19 +708,50 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54AF4425-696E-FE45-90E4-C765F4779314}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -925,18 +966,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70B6D77D-0519-42E5-8A64-FC8C3D3EB3E2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D06517E-E6DE-43DD-A2B3-44E3324281BB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70B6D77D-0519-42E5-8A64-FC8C3D3EB3E2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Fix 919issue [transformer=FROM_EXCEL] Provide possibility to use the range of ALL cells
</commit_message>
<xml_diff>
--- a/vividus-tests/src/main/resources/data/complex-data.xlsx
+++ b/vividus-tests/src/main/resources/data/complex-data.xlsx
@@ -1,22 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/valery_yatsynovich/work/projects/vividus-framework/vividus/vividus-tests/src/main/resources/data/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFEBF766-33B2-224C-BD3B-E3BB0ACCA93B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{E7E63800-A407-481E-BA1A-995B36E7D106}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="480" windowWidth="28800" windowHeight="16660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="23304" windowHeight="13224" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
     <sheet name="with separators" sheetId="2" r:id="rId2"/>
+    <sheet name="range-all-cells" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:O13"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>#</t>
   </si>
@@ -67,6 +64,33 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>date1</t>
+  </si>
+  <si>
+    <t>date2</t>
+  </si>
+  <si>
+    <t>date3</t>
+  </si>
+  <si>
+    <t>line1</t>
+  </si>
+  <si>
+    <t>line2</t>
+  </si>
+  <si>
+    <t>line3</t>
+  </si>
+  <si>
+    <t>line4</t>
+  </si>
+  <si>
+    <t>line5</t>
+  </si>
+  <si>
+    <t>line6</t>
   </si>
 </sst>
 </file>
@@ -550,30 +574,30 @@
   </sheetPr>
   <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+    <sheetView zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.33203125" style="1" customWidth="1"/>
     <col min="3" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="11"/>
     </row>
-    <row r="2" spans="1:2" s="2" customFormat="1" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" s="2" customFormat="1" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="12"/>
     </row>
-    <row r="3" spans="1:2" s="2" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" s="2" customFormat="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -581,7 +605,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="5" customFormat="1" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" s="5" customFormat="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <v>1</v>
       </c>
@@ -589,35 +613,35 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A5" s="9"/>
       <c r="B5" s="6"/>
     </row>
-    <row r="6" spans="1:2" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A6" s="9"/>
       <c r="B6" s="6"/>
     </row>
-    <row r="7" spans="1:2" s="2" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" s="2" customFormat="1" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9"/>
       <c r="B7" s="6"/>
     </row>
-    <row r="8" spans="1:2" s="2" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" s="2" customFormat="1" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9"/>
       <c r="B8" s="6"/>
     </row>
-    <row r="9" spans="1:2" s="2" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" s="2" customFormat="1" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9"/>
       <c r="B9" s="6"/>
     </row>
-    <row r="10" spans="1:2" s="2" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" s="2" customFormat="1" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9"/>
       <c r="B10" s="6"/>
     </row>
-    <row r="11" spans="1:2" s="2" customFormat="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" s="2" customFormat="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="10"/>
       <c r="B11" s="7"/>
     </row>
-    <row r="12" spans="1:2" s="5" customFormat="1" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" s="5" customFormat="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A12" s="8">
         <v>2</v>
       </c>
@@ -625,35 +649,35 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:2" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A13" s="9"/>
       <c r="B13" s="6"/>
     </row>
-    <row r="14" spans="1:2" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A14" s="9"/>
       <c r="B14" s="6"/>
     </row>
-    <row r="15" spans="1:2" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A15" s="9"/>
       <c r="B15" s="6"/>
     </row>
-    <row r="16" spans="1:2" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A16" s="9"/>
       <c r="B16" s="6"/>
     </row>
-    <row r="17" spans="1:2" s="2" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" s="2" customFormat="1" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="9"/>
       <c r="B17" s="6"/>
     </row>
-    <row r="18" spans="1:2" s="2" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" s="2" customFormat="1" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="9"/>
       <c r="B18" s="6"/>
     </row>
-    <row r="19" spans="1:2" s="2" customFormat="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" s="2" customFormat="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="10"/>
       <c r="B19" s="7"/>
     </row>
-    <row r="20" spans="1:2" s="5" customFormat="1" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" s="5" customFormat="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A20" s="8">
         <v>3</v>
       </c>
@@ -661,35 +685,35 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:2" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A21" s="9"/>
       <c r="B21" s="6"/>
     </row>
-    <row r="22" spans="1:2" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A22" s="9"/>
       <c r="B22" s="6"/>
     </row>
-    <row r="23" spans="1:2" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A23" s="9"/>
       <c r="B23" s="6"/>
     </row>
-    <row r="24" spans="1:2" s="2" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" s="2" customFormat="1" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="9"/>
       <c r="B24" s="6"/>
     </row>
-    <row r="25" spans="1:2" s="2" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" s="2" customFormat="1" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="9"/>
       <c r="B25" s="6"/>
     </row>
-    <row r="26" spans="1:2" s="2" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" s="2" customFormat="1" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="9"/>
       <c r="B26" s="6"/>
     </row>
-    <row r="27" spans="1:2" s="2" customFormat="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" s="2" customFormat="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="10"/>
       <c r="B27" s="7"/>
     </row>
-    <row r="28" spans="1:2" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A4:A11"/>
@@ -712,13 +736,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54AF4425-696E-FE45-90E4-C765F4779314}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -726,7 +750,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -739,22 +763,61 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EEE9905-6599-4C8E-BA72-1847904FD80B}">
+  <dimension ref="A2:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E6AB67934BA7844F942979E09252B52C" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="49c38a6fab897aa9265a750643a19c7c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="be478229-e123-4c39-a331-b5c721fb28cc" xmlns:ns3="bc92fd81-69d3-45bd-817e-afa61c088b57" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ce708c13f7346879ef4a91e34fe70bc2" ns2:_="" ns3:_="">
     <xsd:import namespace="be478229-e123-4c39-a331-b5c721fb28cc"/>
@@ -965,24 +1028,22 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70B6D77D-0519-42E5-8A64-FC8C3D3EB3E2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D06517E-E6DE-43DD-A2B3-44E3324281BB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC87063C-09C9-4C6D-B8D3-21213D36F055}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -999,4 +1060,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D06517E-E6DE-43DD-A2B3-44E3324281BB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70B6D77D-0519-42E5-8A64-FC8C3D3EB3E2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[plugin-excel] Add ability to extract full table using FROM_EXCEL transformer (#962)
</commit_message>
<xml_diff>
--- a/vividus-tests/src/main/resources/data/complex-data.xlsx
+++ b/vividus-tests/src/main/resources/data/complex-data.xlsx
@@ -1,22 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/valery_yatsynovich/work/projects/vividus-framework/vividus/vividus-tests/src/main/resources/data/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFEBF766-33B2-224C-BD3B-E3BB0ACCA93B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{E7E63800-A407-481E-BA1A-995B36E7D106}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="480" windowWidth="28800" windowHeight="16660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="23304" windowHeight="13224" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
     <sheet name="with separators" sheetId="2" r:id="rId2"/>
+    <sheet name="range-all-cells" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:O13"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>#</t>
   </si>
@@ -67,6 +64,33 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>date1</t>
+  </si>
+  <si>
+    <t>date2</t>
+  </si>
+  <si>
+    <t>date3</t>
+  </si>
+  <si>
+    <t>line1</t>
+  </si>
+  <si>
+    <t>line2</t>
+  </si>
+  <si>
+    <t>line3</t>
+  </si>
+  <si>
+    <t>line4</t>
+  </si>
+  <si>
+    <t>line5</t>
+  </si>
+  <si>
+    <t>line6</t>
   </si>
 </sst>
 </file>
@@ -550,30 +574,30 @@
   </sheetPr>
   <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+    <sheetView zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.33203125" style="1" customWidth="1"/>
     <col min="3" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="11"/>
     </row>
-    <row r="2" spans="1:2" s="2" customFormat="1" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" s="2" customFormat="1" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="12"/>
     </row>
-    <row r="3" spans="1:2" s="2" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" s="2" customFormat="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -581,7 +605,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="5" customFormat="1" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" s="5" customFormat="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <v>1</v>
       </c>
@@ -589,35 +613,35 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A5" s="9"/>
       <c r="B5" s="6"/>
     </row>
-    <row r="6" spans="1:2" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A6" s="9"/>
       <c r="B6" s="6"/>
     </row>
-    <row r="7" spans="1:2" s="2" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" s="2" customFormat="1" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9"/>
       <c r="B7" s="6"/>
     </row>
-    <row r="8" spans="1:2" s="2" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" s="2" customFormat="1" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9"/>
       <c r="B8" s="6"/>
     </row>
-    <row r="9" spans="1:2" s="2" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" s="2" customFormat="1" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9"/>
       <c r="B9" s="6"/>
     </row>
-    <row r="10" spans="1:2" s="2" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" s="2" customFormat="1" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9"/>
       <c r="B10" s="6"/>
     </row>
-    <row r="11" spans="1:2" s="2" customFormat="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" s="2" customFormat="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="10"/>
       <c r="B11" s="7"/>
     </row>
-    <row r="12" spans="1:2" s="5" customFormat="1" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" s="5" customFormat="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A12" s="8">
         <v>2</v>
       </c>
@@ -625,35 +649,35 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:2" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A13" s="9"/>
       <c r="B13" s="6"/>
     </row>
-    <row r="14" spans="1:2" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A14" s="9"/>
       <c r="B14" s="6"/>
     </row>
-    <row r="15" spans="1:2" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A15" s="9"/>
       <c r="B15" s="6"/>
     </row>
-    <row r="16" spans="1:2" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A16" s="9"/>
       <c r="B16" s="6"/>
     </row>
-    <row r="17" spans="1:2" s="2" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" s="2" customFormat="1" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="9"/>
       <c r="B17" s="6"/>
     </row>
-    <row r="18" spans="1:2" s="2" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" s="2" customFormat="1" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="9"/>
       <c r="B18" s="6"/>
     </row>
-    <row r="19" spans="1:2" s="2" customFormat="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" s="2" customFormat="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="10"/>
       <c r="B19" s="7"/>
     </row>
-    <row r="20" spans="1:2" s="5" customFormat="1" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" s="5" customFormat="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A20" s="8">
         <v>3</v>
       </c>
@@ -661,35 +685,35 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:2" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A21" s="9"/>
       <c r="B21" s="6"/>
     </row>
-    <row r="22" spans="1:2" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A22" s="9"/>
       <c r="B22" s="6"/>
     </row>
-    <row r="23" spans="1:2" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A23" s="9"/>
       <c r="B23" s="6"/>
     </row>
-    <row r="24" spans="1:2" s="2" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" s="2" customFormat="1" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="9"/>
       <c r="B24" s="6"/>
     </row>
-    <row r="25" spans="1:2" s="2" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" s="2" customFormat="1" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="9"/>
       <c r="B25" s="6"/>
     </row>
-    <row r="26" spans="1:2" s="2" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" s="2" customFormat="1" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="9"/>
       <c r="B26" s="6"/>
     </row>
-    <row r="27" spans="1:2" s="2" customFormat="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" s="2" customFormat="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="10"/>
       <c r="B27" s="7"/>
     </row>
-    <row r="28" spans="1:2" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A4:A11"/>
@@ -712,13 +736,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54AF4425-696E-FE45-90E4-C765F4779314}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -726,7 +750,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -739,22 +763,61 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EEE9905-6599-4C8E-BA72-1847904FD80B}">
+  <dimension ref="A2:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E6AB67934BA7844F942979E09252B52C" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="49c38a6fab897aa9265a750643a19c7c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="be478229-e123-4c39-a331-b5c721fb28cc" xmlns:ns3="bc92fd81-69d3-45bd-817e-afa61c088b57" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ce708c13f7346879ef4a91e34fe70bc2" ns2:_="" ns3:_="">
     <xsd:import namespace="be478229-e123-4c39-a331-b5c721fb28cc"/>
@@ -965,24 +1028,22 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70B6D77D-0519-42E5-8A64-FC8C3D3EB3E2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D06517E-E6DE-43DD-A2B3-44E3324281BB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC87063C-09C9-4C6D-B8D3-21213D36F055}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -999,4 +1060,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D06517E-E6DE-43DD-A2B3-44E3324281BB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70B6D77D-0519-42E5-8A64-FC8C3D3EB3E2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>